<commit_message>
Adapt programes for the preparation of edition 2403
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,15 +487,23 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mara Sattei</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mare Aperto</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -505,32 +513,40 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" t="n">
-        <v>2.20055888328147</v>
+        <v>-3.680385838987013</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Artemas</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>i like the way you kiss me</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -540,67 +556,83 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="n">
-        <v>5.217145173321046</v>
+        <v>-0.1339579018612671</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Estonia</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>Latvia</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MADARA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Es Esmu Viss</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>6.224033545811571</v>
+        <v>4.207078227973158</v>
       </c>
       <c r="J4" t="n">
         <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Darin</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -610,194 +642,234 @@
         <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I5" t="n">
-        <v>7.99291430207882</v>
+        <v>4.497742459782174</v>
       </c>
       <c r="J5" t="n">
         <v>4</v>
       </c>
       <c r="K5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Andorra</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Luka</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>9</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.043921043641335</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
         <v>4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7</v>
-      </c>
-      <c r="I6" t="n">
-        <v>9.019696782165164</v>
-      </c>
-      <c r="J6" t="n">
-        <v>5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>Albania</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Yll Limani</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Buzet e kuqe</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.416131930182489</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" t="n">
         <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>13</v>
-      </c>
-      <c r="H7" t="n">
-        <v>20</v>
-      </c>
-      <c r="I7" t="n">
-        <v>9.392886627101053</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Agoney</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tormenta</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
         <v>8</v>
       </c>
-      <c r="H8" t="n">
-        <v>22</v>
-      </c>
       <c r="I8" t="n">
-        <v>10.22764672240861</v>
+        <v>5.482876354397287</v>
       </c>
       <c r="J8" t="n">
         <v>7</v>
       </c>
       <c r="K8" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Denmark</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Fernando Daniel</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>casa</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="I9" t="n">
-        <v>10.57922150072928</v>
+        <v>5.506493421366757</v>
       </c>
       <c r="J9" t="n">
         <v>8</v>
       </c>
       <c r="K9" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Romania</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+          <t>San Marino</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ALFA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Vai!</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I10" t="n">
-        <v>11.15607106454494</v>
+        <v>6.366751796905027</v>
       </c>
       <c r="J10" t="n">
         <v>9</v>
       </c>
       <c r="K10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -806,27 +878,35 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Albania</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Dami Im</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Collide</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>11.68721309541866</v>
+        <v>6.477241395333476</v>
       </c>
       <c r="J11" t="n">
         <v>10</v>
@@ -837,190 +917,238 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Azerbaijan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AISEL</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Game of Chess</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>EMSC 2402</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" t="n">
         <v>2</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Morocco</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" t="n">
-        <v>6</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3</v>
-      </c>
       <c r="I12" t="n">
-        <v>11.91301209194449</v>
+        <v>6.552457415670258</v>
       </c>
       <c r="J12" t="n">
         <v>11</v>
       </c>
       <c r="K12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ireland</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Thorsteinn Einarsson</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Hotel Heartache</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I13" t="n">
-        <v>12.56542713843339</v>
+        <v>6.845252141928177</v>
       </c>
       <c r="J13" t="n">
         <v>12</v>
       </c>
       <c r="K13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SERA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Head Held High</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G14" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H14" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I14" t="n">
-        <v>13.07123339416382</v>
+        <v>7.674800272907581</v>
       </c>
       <c r="J14" t="n">
         <v>13</v>
       </c>
       <c r="K14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nigeria</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SARA'H</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TU PARLES</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G15" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="H15" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I15" t="n">
-        <v>13.24665544364137</v>
+        <v>8.077167957355112</v>
       </c>
       <c r="J15" t="n">
         <v>14</v>
       </c>
       <c r="K15" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Tamara Todevska</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Monsters</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G16" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H16" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I16" t="n">
-        <v>14.60941914692027</v>
+        <v>8.528833102917558</v>
       </c>
       <c r="J16" t="n">
         <v>15</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>HUNGER</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>HONEY</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1030,135 +1158,165 @@
         <v>9</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H17" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I17" t="n">
-        <v>14.97960964925794</v>
+        <v>11.31149238989227</v>
       </c>
       <c r="J17" t="n">
         <v>16</v>
       </c>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+          <t>Israel</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Yam Rafaeli ft. Orr Amrami Brockman</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Teruf</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I18" t="n">
-        <v>15.27343480452621</v>
+        <v>11.46733896008557</v>
       </c>
       <c r="J18" t="n">
         <v>17</v>
       </c>
       <c r="K18" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+          <t>Croatia</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Top of the Pop ft. Mario 5reković</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Putovanje</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I19" t="n">
-        <v>15.40379115430613</v>
+        <v>12.5334498401962</v>
       </c>
       <c r="J19" t="n">
         <v>18</v>
       </c>
       <c r="K19" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>San Marino</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+          <t>Türkiye</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>INJI</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>BELLYDANCING</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>11</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="n">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>15.62101617649303</v>
+        <v>12.81319403984015</v>
       </c>
       <c r="J20" t="n">
         <v>19</v>
       </c>
-      <c r="K20" t="n">
-        <v>9</v>
-      </c>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Austria</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ana Mena, GALE</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>La Razón</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1168,120 +1326,148 @@
         <v>8</v>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H21" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I21" t="n">
-        <v>15.84278048560179</v>
+        <v>13.68329608768173</v>
       </c>
       <c r="J21" t="n">
         <v>20</v>
       </c>
       <c r="K21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Greece</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+          <t>Bulgaria</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ALMA x Kristian Kostov</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>So High</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5</v>
+      </c>
       <c r="H22" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I22" t="n">
-        <v>18.02733026490223</v>
+        <v>15.05952238805769</v>
       </c>
       <c r="J22" t="n">
         <v>21</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>TVORCHI</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Shine</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>EMSC 2402</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>12</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Malta</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>7</v>
-      </c>
       <c r="G23" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H23" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I23" t="n">
-        <v>18.54762833014271</v>
+        <v>15.21434765249735</v>
       </c>
       <c r="J23" t="n">
         <v>22</v>
       </c>
       <c r="K23" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Japan</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>I Was Gonna Marry Him</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>EYJAA</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>12</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9</v>
+      </c>
       <c r="H24" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I24" t="n">
-        <v>19.1175988851479</v>
+        <v>16.09186603086978</v>
       </c>
       <c r="J24" t="n">
         <v>23</v>
       </c>
       <c r="K24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1290,11 +1476,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Chile</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+          <t>Armenia</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Lilit Hovhannisyan &amp; GASOIIA</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Ush a</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1303,10 +1497,12 @@
       <c r="F25" t="n">
         <v>13</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>5</v>
+      </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>21.14056352376259</v>
+        <v>17.29360470218849</v>
       </c>
       <c r="J25" t="n">
         <v>24</v>
@@ -1315,65 +1511,89 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Norway</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Hozier</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Too Sweet</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>12</v>
-      </c>
-      <c r="G26" t="inlineStr"/>
+        <v>9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>18</v>
+      </c>
       <c r="H26" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I26" t="n">
-        <v>21.99488145705836</v>
+        <v>18.73508444380843</v>
       </c>
       <c r="J26" t="n">
         <v>25</v>
       </c>
       <c r="K26" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MIRA</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bad Booty</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>15</v>
-      </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>17</v>
+      </c>
       <c r="I27" t="n">
-        <v>22.32768822922124</v>
+        <v>19.64891562532673</v>
       </c>
       <c r="J27" t="n">
         <v>26</v>
       </c>
-      <c r="K27" t="inlineStr"/>
+      <c r="K27" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1381,11 +1601,19 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+          <t>Cyprus</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ivi Adamou</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Eipes</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1394,10 +1622,12 @@
       <c r="F28" t="n">
         <v>13</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>5</v>
+      </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>22.76004084640601</v>
+        <v>19.85142992058191</v>
       </c>
       <c r="J28" t="n">
         <v>27</v>
@@ -1406,27 +1636,37 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Wincent Weiss</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Wo die Liebe hinfällt</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>14</v>
-      </c>
-      <c r="G29" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5</v>
+      </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>22.85345918995974</v>
+        <v>21.25481368860495</v>
       </c>
       <c r="J29" t="n">
         <v>28</v>
@@ -1439,11 +1679,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Colombia</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+          <t>Serbia</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>BRESKVICA</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LEPTIR</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1452,10 +1700,12 @@
       <c r="F30" t="n">
         <v>16</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>5</v>
+      </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>24.75643099687996</v>
+        <v>21.84349194840515</v>
       </c>
       <c r="J30" t="n">
         <v>29</v>
@@ -1464,27 +1714,37 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Monaco</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+          <t>Morocco</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Amel Bent x DADJU</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Tu l’aimes encore</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>17</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>25.57627687912843</v>
+        <v>22.81351816409759</v>
       </c>
       <c r="J31" t="n">
         <v>30</v>
@@ -1493,27 +1753,37 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Philippines</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+          <t>Finland</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Käärijä x Erika Vikman</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Ruoska</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>16</v>
-      </c>
-      <c r="G32" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5</v>
+      </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>25.67847025891104</v>
+        <v>24.83932593283525</v>
       </c>
       <c r="J32" t="n">
         <v>31</v>
@@ -1522,27 +1792,37 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>St Graal</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Drag</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>15</v>
-      </c>
-      <c r="G33" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5</v>
+      </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>26.29927981437986</v>
+        <v>24.96037440019548</v>
       </c>
       <c r="J33" t="n">
         <v>32</v>
@@ -1551,15 +1831,23 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Hungary</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+          <t>Slovenia</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Žan Serčič</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bela Lilija</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>EMSC 2402</t>
@@ -1568,15 +1856,95 @@
       <c r="F34" t="n">
         <v>14</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>5</v>
+      </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>26.92681778399507</v>
+        <v>25.89750180405654</v>
       </c>
       <c r="J34" t="n">
         <v>33</v>
       </c>
       <c r="K34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Montenegro</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Bojan Marović</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Živjeti za nas</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EMSC 2402</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>18</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5</v>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>28.4036391551474</v>
+      </c>
+      <c r="J35" t="n">
+        <v>34</v>
+      </c>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Nutsa Buzaladze</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>A Mother’s Love</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>EMSC 2402</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>14</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5</v>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>28.92617981832787</v>
+      </c>
+      <c r="J36" t="n">
+        <v>35</v>
+      </c>
+      <c r="K36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update stats to accomodate edition 2404
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,50 +487,50 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Azerbaijan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Artemas</t>
+          <t>SEVDALIZA FT. PABLLO VITTAR &amp; YSEULT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>i like the way you kiss me</t>
+          <t>ALIBI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H2" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" t="n">
-        <v>1.610065659202821</v>
+        <v>2.670303786386871</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -539,983 +539,1308 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mara Sattei</t>
+          <t>Coma_Cose</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mare Aperto</t>
+          <t>MALAVITA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I3" t="n">
-        <v>4.377729292645222</v>
+        <v>3.168547184156584</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yll Limani</t>
+          <t>Aden Foyer</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Buzet e kuqe</t>
+          <t>Galileo Galilei</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I4" t="n">
-        <v>5.308210830983475</v>
+        <v>4.476878941770735</v>
       </c>
       <c r="J4" t="n">
         <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fernando Daniel</t>
+          <t>Hannah Mae &amp; Maksim</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>casa</t>
+          <t>Ik Wil Dat Je Liegt</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>6.310688766102115</v>
+        <v>6.090991511331351</v>
       </c>
       <c r="J5" t="n">
         <v>4</v>
       </c>
       <c r="K5" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Thorsteinn Einarsson</t>
+          <t>Javy Ramírez</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hotel Heartache</t>
+          <t>Tu Nombre</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" t="n">
-        <v>7.117627613302684</v>
+        <v>9.48077520576458</v>
       </c>
       <c r="J6" t="n">
         <v>5</v>
       </c>
       <c r="K6" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Darin</t>
+          <t>VIKTORIO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Electric</t>
+          <t>Tough To Love</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H7" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I7" t="n">
-        <v>9.358608574544572</v>
+        <v>9.774776981983475</v>
       </c>
       <c r="J7" t="n">
         <v>6</v>
       </c>
       <c r="K7" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALMA x Kristian Kostov</t>
+          <t>Aimée</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>So High</t>
+          <t>Daisy Chains</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H8" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I8" t="n">
-        <v>10.49241536455297</v>
+        <v>10.25323105081258</v>
       </c>
       <c r="J8" t="n">
         <v>7</v>
       </c>
       <c r="K8" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dami Im</t>
+          <t>Niam</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Collide</t>
+          <t>guignols</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
-        <v>11.65683980004958</v>
+        <v>11.11748275777789</v>
       </c>
       <c r="J9" t="n">
         <v>8</v>
       </c>
       <c r="K9" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Croatia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Nina Badric</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Kako si</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>6</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>North Macedonia</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Tamara Todevska</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Monsters</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>7</v>
-      </c>
       <c r="G10" t="n">
+        <v>23</v>
+      </c>
+      <c r="H10" t="n">
         <v>2</v>
       </c>
-      <c r="H10" t="n">
-        <v>7</v>
-      </c>
       <c r="I10" t="n">
-        <v>11.96195256035154</v>
+        <v>11.33734360927431</v>
       </c>
       <c r="J10" t="n">
         <v>9</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>San Marino</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Agoney</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Tormenta</t>
+          <t>IL BENE NEL MALE</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G11" t="n">
         <v>18</v>
       </c>
       <c r="H11" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I11" t="n">
-        <v>13.02670484600449</v>
+        <v>11.38709368843426</v>
       </c>
       <c r="J11" t="n">
         <v>10</v>
       </c>
       <c r="K11" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>San Marino</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ALFA</t>
+          <t>Sofia Camara</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Vai!</t>
+          <t>Who Do I Call Now?</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" t="n">
         <v>6</v>
       </c>
-      <c r="G12" t="n">
-        <v>16</v>
-      </c>
-      <c r="H12" t="n">
-        <v>14</v>
-      </c>
       <c r="I12" t="n">
-        <v>13.22153846794309</v>
+        <v>11.86212022621625</v>
       </c>
       <c r="J12" t="n">
         <v>11</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Luka</t>
+          <t>Nikos Oikonomopoulos</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FOMO</t>
+          <t>Valto Terma</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I13" t="n">
-        <v>13.29296108155018</v>
+        <v>12.36796797335973</v>
       </c>
       <c r="J13" t="n">
         <v>12</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Türkiye</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HUNGER</t>
+          <t>Ziynet Sali</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HONEY</t>
+          <t>Daha Nasıl Sevebilirim</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>9</v>
-      </c>
-      <c r="G14" t="n">
-        <v>10</v>
-      </c>
-      <c r="H14" t="n">
-        <v>4</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>13.7458335309414</v>
+        <v>13.17061176623693</v>
       </c>
       <c r="J14" t="n">
         <v>13</v>
       </c>
-      <c r="K14" t="n">
-        <v>9</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Andorra</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ana Mena, GALE</t>
+          <t>Narkis</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>La Razón</t>
+          <t>הכל לטובה</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H15" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I15" t="n">
-        <v>13.98732754746183</v>
+        <v>13.42390690753203</v>
       </c>
       <c r="J15" t="n">
         <v>14</v>
       </c>
       <c r="K15" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MIRA</t>
+          <t>Elhaida Dani</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bad Booty</t>
+          <t>Zemrës</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7</v>
+      </c>
+      <c r="H16" t="n">
         <v>12</v>
       </c>
-      <c r="G16" t="n">
-        <v>6</v>
-      </c>
-      <c r="H16" t="n">
-        <v>17</v>
-      </c>
       <c r="I16" t="n">
-        <v>15.04667844579388</v>
+        <v>13.63229694219903</v>
       </c>
       <c r="J16" t="n">
         <v>15</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Monaco</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SERA</t>
+          <t>Lukas Abdul</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Head Held High</t>
+          <t>Les Maux Bleus</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G17" t="n">
         <v>22</v>
       </c>
       <c r="H17" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I17" t="n">
-        <v>15.14069794897265</v>
+        <v>13.77239263451249</v>
       </c>
       <c r="J17" t="n">
         <v>16</v>
       </c>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Czechia</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SARA'H</t>
+          <t>MIKOLAS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>TU PARLES</t>
+          <t>DELILAH</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G18" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="H18" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>15.70331226722626</v>
+        <v>13.84377701635244</v>
       </c>
       <c r="J18" t="n">
         <v>17</v>
       </c>
       <c r="K18" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Hozier</t>
+          <t>Gregor Hägele</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Too Sweet</t>
+          <t>1 Jahr</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>9</v>
       </c>
       <c r="G19" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H19" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I19" t="n">
-        <v>15.71802745189748</v>
+        <v>14.47791392816426</v>
       </c>
       <c r="J19" t="n">
         <v>18</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Husavik</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>My Home Town</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>9</v>
+      </c>
+      <c r="G20" t="n">
         <v>2</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Latvia</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MADARA</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Es Esmu Viss</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
+      <c r="H20" t="n">
         <v>8</v>
       </c>
-      <c r="G20" t="n">
-        <v>4</v>
-      </c>
-      <c r="H20" t="n">
-        <v>3</v>
-      </c>
       <c r="I20" t="n">
-        <v>16.36966782701744</v>
+        <v>14.51945743817884</v>
       </c>
       <c r="J20" t="n">
         <v>19</v>
       </c>
       <c r="K20" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>I Was Gonna Marry Him</t>
+          <t>ABREU</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>EYJAA</t>
+          <t>Caliente</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G21" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H21" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I21" t="n">
-        <v>18.211610326263</v>
+        <v>14.90715299786459</v>
       </c>
       <c r="J21" t="n">
         <v>20</v>
       </c>
       <c r="K21" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Maro</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>HELLSTORM</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>11</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Israel</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Yam Rafaeli ft. Orr Amrami Brockman</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Teruf</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>10</v>
-      </c>
       <c r="G22" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H22" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I22" t="n">
-        <v>18.7034332541139</v>
+        <v>17.85156633112051</v>
       </c>
       <c r="J22" t="n">
         <v>21</v>
       </c>
       <c r="K22" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Melissa Naschenweng</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Legenden</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>12</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Croatia</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Top of the Pop ft. Mario 5reković</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Putovanje</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>EMSC 2402</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
+        <v>5</v>
+      </c>
+      <c r="H23" t="n">
         <v>10</v>
       </c>
-      <c r="G23" t="n">
-        <v>13</v>
-      </c>
-      <c r="H23" t="n">
-        <v>13</v>
-      </c>
       <c r="I23" t="n">
-        <v>18.970220432375</v>
+        <v>18.57963432069638</v>
       </c>
       <c r="J23" t="n">
         <v>22</v>
       </c>
       <c r="K23" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Azerbaijan</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AISEL</t>
+          <t>Marija Serifovic feat. Matija Cvek</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Game of Chess</t>
+          <t>POLA SUNCA</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>11</v>
       </c>
       <c r="G24" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="I24" t="n">
-        <v>20.25692200043978</v>
+        <v>18.97039007004728</v>
       </c>
       <c r="J24" t="n">
         <v>23</v>
       </c>
       <c r="K24" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TVORCHI</t>
+          <t>Taska Black</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Shine</t>
+          <t>Comedown</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>EMSC 2402</t>
+          <t>EMSC 2403</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G25" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H25" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I25" t="n">
-        <v>22.7086890414944</v>
+        <v>20.95134238969322</v>
       </c>
       <c r="J25" t="n">
         <v>24</v>
       </c>
       <c r="K25" t="n">
-        <v>19</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Basim</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Johnny</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>14</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>21.8612342112588</v>
+      </c>
+      <c r="J26" t="n">
+        <v>25</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Greece</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ZAF</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MAXH</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>13</v>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>22.388379215675</v>
+      </c>
+      <c r="J27" t="n">
+        <v>26</v>
+      </c>
+      <c r="K27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>15</v>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>23.12885717662297</v>
+      </c>
+      <c r="J28" t="n">
+        <v>27</v>
+      </c>
+      <c r="K28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>DePol</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Dime solo si has pensao</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>13</v>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>23.16733609117585</v>
+      </c>
+      <c r="J29" t="n">
+        <v>28</v>
+      </c>
+      <c r="K29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>dEUS</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Faux Bamboo</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>15</v>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>25.21799372444785</v>
+      </c>
+      <c r="J30" t="n">
+        <v>29</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Rawanne X Dj Jackson</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Punjabi</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>16</v>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>25.34033430507186</v>
+      </c>
+      <c r="J31" t="n">
+        <v>30</v>
+      </c>
+      <c r="K31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Switzerland</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Luca Hänni</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Stay With Me</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>12</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4</v>
+      </c>
+      <c r="H32" t="n">
+        <v>21</v>
+      </c>
+      <c r="I32" t="n">
+        <v>26.19225410483391</v>
+      </c>
+      <c r="J32" t="n">
+        <v>31</v>
+      </c>
+      <c r="K32" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Tunisia</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>MYRATH</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Heroes</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>16</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>26.19518090571541</v>
+      </c>
+      <c r="J33" t="n">
+        <v>32</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>flowerkid</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>vodka orange juice</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>EMSC 2403</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>17</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>30.07017329799616</v>
+      </c>
+      <c r="J34" t="n">
+        <v>33</v>
+      </c>
+      <c r="K34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>